<commit_message>
Final Functionality changes and algorithm implementation
</commit_message>
<xml_diff>
--- a/zzzzz/chitwan.xlsx
+++ b/zzzzz/chitwan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ishan\OneDrive\Desktop\Dine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ishan\OneDrive\Desktop\Dine\zzzzz\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="chitwan" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1197" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="509">
   <si>
     <t>URL</t>
   </si>
@@ -1543,6 +1543,9 @@
   </si>
   <si>
     <t>Closes 8PM</t>
+  </si>
+  <si>
+    <t>restaurant-id</t>
   </si>
 </sst>
 </file>
@@ -2349,15 +2352,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L121"/>
+  <dimension ref="A1:M121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
     <col min="5" max="5" width="22.28515625" customWidth="1"/>
     <col min="6" max="6" width="29.5703125" customWidth="1"/>
     <col min="7" max="7" width="37.7109375" customWidth="1"/>
@@ -2368,7 +2374,7 @@
     <col min="12" max="12" width="51.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2405,8 +2411,11 @@
       <c r="L1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2443,8 +2452,11 @@
       <c r="L2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -2481,8 +2493,11 @@
       <c r="L3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -2516,8 +2531,11 @@
       <c r="L4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -2554,8 +2572,11 @@
       <c r="L5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -2592,8 +2613,11 @@
       <c r="L6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -2630,8 +2654,11 @@
       <c r="L7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -2665,8 +2692,11 @@
       <c r="L8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -2703,8 +2733,11 @@
       <c r="L9" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -2741,8 +2774,11 @@
       <c r="L10" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -2779,8 +2815,11 @@
       <c r="L11" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -2817,8 +2856,11 @@
       <c r="L12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -2855,8 +2897,11 @@
       <c r="L13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -2893,8 +2938,11 @@
       <c r="L14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -2931,8 +2979,11 @@
       <c r="L15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>73</v>
       </c>
@@ -2969,8 +3020,11 @@
       <c r="L16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>78</v>
       </c>
@@ -3004,8 +3058,11 @@
       <c r="L17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>81</v>
       </c>
@@ -3042,8 +3099,11 @@
       <c r="L18" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>85</v>
       </c>
@@ -3080,8 +3140,11 @@
       <c r="L19" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>89</v>
       </c>
@@ -3118,8 +3181,11 @@
       <c r="L20" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>93</v>
       </c>
@@ -3156,8 +3222,11 @@
       <c r="L21" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>97</v>
       </c>
@@ -3194,8 +3263,11 @@
       <c r="L22" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>101</v>
       </c>
@@ -3232,8 +3304,11 @@
       <c r="L23" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>105</v>
       </c>
@@ -3270,8 +3345,11 @@
       <c r="L24" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>109</v>
       </c>
@@ -3308,8 +3386,11 @@
       <c r="L25" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>114</v>
       </c>
@@ -3346,8 +3427,11 @@
       <c r="L26" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>118</v>
       </c>
@@ -3384,8 +3468,11 @@
       <c r="L27" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>122</v>
       </c>
@@ -3422,8 +3509,11 @@
       <c r="L28" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>127</v>
       </c>
@@ -3460,8 +3550,11 @@
       <c r="L29" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>131</v>
       </c>
@@ -3498,8 +3591,11 @@
       <c r="L30" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>135</v>
       </c>
@@ -3536,8 +3632,11 @@
       <c r="L31" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>139</v>
       </c>
@@ -3574,8 +3673,11 @@
       <c r="L32" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>143</v>
       </c>
@@ -3612,8 +3714,11 @@
       <c r="L33" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>148</v>
       </c>
@@ -3647,8 +3752,11 @@
       <c r="L34" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>151</v>
       </c>
@@ -3685,8 +3793,11 @@
       <c r="L35" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>155</v>
       </c>
@@ -3723,8 +3834,11 @@
       <c r="L36" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>160</v>
       </c>
@@ -3761,8 +3875,11 @@
       <c r="L37" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>164</v>
       </c>
@@ -3799,8 +3916,11 @@
       <c r="L38" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>168</v>
       </c>
@@ -3837,8 +3957,11 @@
       <c r="L39" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>172</v>
       </c>
@@ -3875,8 +3998,11 @@
       <c r="L40" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>176</v>
       </c>
@@ -3913,8 +4039,11 @@
       <c r="L41" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>180</v>
       </c>
@@ -3951,8 +4080,11 @@
       <c r="L42" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>184</v>
       </c>
@@ -3989,8 +4121,11 @@
       <c r="L43" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>188</v>
       </c>
@@ -4027,8 +4162,11 @@
       <c r="L44" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>193</v>
       </c>
@@ -4065,8 +4203,11 @@
       <c r="L45" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>197</v>
       </c>
@@ -4103,8 +4244,11 @@
       <c r="L46" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>201</v>
       </c>
@@ -4138,8 +4282,11 @@
       <c r="L47" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>204</v>
       </c>
@@ -4176,8 +4323,11 @@
       <c r="L48" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>208</v>
       </c>
@@ -4214,8 +4364,11 @@
       <c r="L49" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>212</v>
       </c>
@@ -4249,8 +4402,11 @@
       <c r="L50" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>215</v>
       </c>
@@ -4287,8 +4443,11 @@
       <c r="L51" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>219</v>
       </c>
@@ -4325,8 +4484,11 @@
       <c r="L52" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>223</v>
       </c>
@@ -4360,8 +4522,11 @@
       <c r="L53" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>226</v>
       </c>
@@ -4395,8 +4560,11 @@
       <c r="L54" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>228</v>
       </c>
@@ -4433,8 +4601,11 @@
       <c r="L55" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>231</v>
       </c>
@@ -4471,8 +4642,11 @@
       <c r="L56" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>235</v>
       </c>
@@ -4509,8 +4683,11 @@
       <c r="L57" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>239</v>
       </c>
@@ -4547,8 +4724,11 @@
       <c r="L58" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>243</v>
       </c>
@@ -4585,8 +4765,11 @@
       <c r="L59" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M59">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>247</v>
       </c>
@@ -4620,8 +4803,11 @@
       <c r="L60" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M60">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>251</v>
       </c>
@@ -4658,8 +4844,11 @@
       <c r="L61" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>255</v>
       </c>
@@ -4696,8 +4885,11 @@
       <c r="L62" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>258</v>
       </c>
@@ -4734,8 +4926,11 @@
       <c r="L63" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>262</v>
       </c>
@@ -4772,8 +4967,11 @@
       <c r="L64" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M64">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>266</v>
       </c>
@@ -4810,8 +5008,11 @@
       <c r="L65" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M65">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>270</v>
       </c>
@@ -4848,8 +5049,11 @@
       <c r="L66" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M66">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>272</v>
       </c>
@@ -4886,8 +5090,11 @@
       <c r="L67" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M67">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>276</v>
       </c>
@@ -4924,8 +5131,11 @@
       <c r="L68" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M68">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>279</v>
       </c>
@@ -4962,8 +5172,11 @@
       <c r="L69" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M69">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>283</v>
       </c>
@@ -5000,8 +5213,11 @@
       <c r="L70" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M70">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>287</v>
       </c>
@@ -5038,8 +5254,11 @@
       <c r="L71" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M71">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>290</v>
       </c>
@@ -5076,8 +5295,11 @@
       <c r="L72" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M72">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>294</v>
       </c>
@@ -5114,8 +5336,11 @@
       <c r="L73" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M73">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>298</v>
       </c>
@@ -5152,8 +5377,11 @@
       <c r="L74" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M74">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>302</v>
       </c>
@@ -5190,8 +5418,11 @@
       <c r="L75" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>306</v>
       </c>
@@ -5228,8 +5459,11 @@
       <c r="L76" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M76">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>310</v>
       </c>
@@ -5266,8 +5500,11 @@
       <c r="L77" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M77">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>314</v>
       </c>
@@ -5301,8 +5538,11 @@
       <c r="L78" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M78">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>317</v>
       </c>
@@ -5339,8 +5579,11 @@
       <c r="L79" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M79">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>321</v>
       </c>
@@ -5377,8 +5620,11 @@
       <c r="L80" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M80">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>325</v>
       </c>
@@ -5415,8 +5661,11 @@
       <c r="L81" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M81">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>329</v>
       </c>
@@ -5453,8 +5702,11 @@
       <c r="L82" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M82">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>333</v>
       </c>
@@ -5488,8 +5740,11 @@
       <c r="L83" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M83">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>336</v>
       </c>
@@ -5526,8 +5781,11 @@
       <c r="L84" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M84">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>339</v>
       </c>
@@ -5564,8 +5822,11 @@
       <c r="L85" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M85">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>343</v>
       </c>
@@ -5602,8 +5863,11 @@
       <c r="L86" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M86">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>347</v>
       </c>
@@ -5640,8 +5904,11 @@
       <c r="L87" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M87">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>351</v>
       </c>
@@ -5678,8 +5945,11 @@
       <c r="L88" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M88">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>355</v>
       </c>
@@ -5716,8 +5986,11 @@
       <c r="L89" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M89">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>359</v>
       </c>
@@ -5754,8 +6027,11 @@
       <c r="L90" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M90">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>363</v>
       </c>
@@ -5792,8 +6068,11 @@
       <c r="L91" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M91">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>367</v>
       </c>
@@ -5830,8 +6109,11 @@
       <c r="L92" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M92">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>371</v>
       </c>
@@ -5868,8 +6150,11 @@
       <c r="L93" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M93">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>375</v>
       </c>
@@ -5906,8 +6191,11 @@
       <c r="L94" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M94">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>379</v>
       </c>
@@ -5944,8 +6232,11 @@
       <c r="L95" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M95">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>383</v>
       </c>
@@ -5982,8 +6273,11 @@
       <c r="L96" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M96">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>386</v>
       </c>
@@ -6020,8 +6314,11 @@
       <c r="L97" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M97">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>390</v>
       </c>
@@ -6058,8 +6355,11 @@
       <c r="L98" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M98">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>394</v>
       </c>
@@ -6096,8 +6396,11 @@
       <c r="L99" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M99">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>398</v>
       </c>
@@ -6134,8 +6437,11 @@
       <c r="L100" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M100">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>403</v>
       </c>
@@ -6172,8 +6478,11 @@
       <c r="L101" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M101">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>406</v>
       </c>
@@ -6210,8 +6519,11 @@
       <c r="L102" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M102">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>410</v>
       </c>
@@ -6245,8 +6557,11 @@
       <c r="L103" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M103">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>411</v>
       </c>
@@ -6283,8 +6598,11 @@
       <c r="L104" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M104">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>414</v>
       </c>
@@ -6321,8 +6639,11 @@
       <c r="L105" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M105">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>417</v>
       </c>
@@ -6359,8 +6680,11 @@
       <c r="L106" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M106">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>420</v>
       </c>
@@ -6397,8 +6721,11 @@
       <c r="L107" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M107">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>423</v>
       </c>
@@ -6432,8 +6759,11 @@
       <c r="L108" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M108">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>426</v>
       </c>
@@ -6470,8 +6800,11 @@
       <c r="L109" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M109">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>430</v>
       </c>
@@ -6508,8 +6841,11 @@
       <c r="L110" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M110">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>434</v>
       </c>
@@ -6546,8 +6882,11 @@
       <c r="L111" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M111">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>438</v>
       </c>
@@ -6584,8 +6923,11 @@
       <c r="L112" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M112">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>442</v>
       </c>
@@ -6619,8 +6961,11 @@
       <c r="L113" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M113">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>445</v>
       </c>
@@ -6657,8 +7002,11 @@
       <c r="L114" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M114">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>448</v>
       </c>
@@ -6695,8 +7043,11 @@
       <c r="L115" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M115">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>452</v>
       </c>
@@ -6733,8 +7084,11 @@
       <c r="L116" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M116">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>456</v>
       </c>
@@ -6771,8 +7125,11 @@
       <c r="L117" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M117">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>460</v>
       </c>
@@ -6809,8 +7166,11 @@
       <c r="L118" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M118">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>464</v>
       </c>
@@ -6847,8 +7207,11 @@
       <c r="L119" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M119">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>468</v>
       </c>
@@ -6882,8 +7245,11 @@
       <c r="L120" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M120">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>471</v>
       </c>
@@ -6919,6 +7285,9 @@
       </c>
       <c r="L121" t="s">
         <v>31</v>
+      </c>
+      <c r="M121">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>